<commit_message>
5th test case added to BOA app
</commit_message>
<xml_diff>
--- a/com.bankofamerica.com/src/test/resources/boaTestData.xlsx
+++ b/com.bankofamerica.com/src/test/resources/boaTestData.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nahid\IdeaProjects\Team5WDESeleniumBootcamp\com.bankofamerica.com\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1353E727-AA1F-4AA7-9C98-620FAAADD135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F5AD7F-B44C-4E6D-9EA5-3178BD316C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{5B3D6E91-87A4-427A-B005-9C27CF189E9B}"/>
   </bookViews>
   <sheets>
-    <sheet name="expedia" sheetId="1" r:id="rId1"/>
-    <sheet name="boaSignup" sheetId="2" r:id="rId2"/>
+    <sheet name="boaSignup" sheetId="2" r:id="rId1"/>
+    <sheet name="loginNegativeTest" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,19 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
-  <si>
-    <t>LocationToSearch</t>
-  </si>
-  <si>
-    <t>CheckInDate</t>
-  </si>
-  <si>
-    <t>CheckOutDate</t>
-  </si>
-  <si>
-    <t>Dhaka (DAC - Shahjalal Intl.)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>email</t>
   </si>
@@ -83,6 +71,33 @@
   </si>
   <si>
     <t>Muhammad</t>
+  </si>
+  <si>
+    <t>OnlineId</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ABCDE</t>
+  </si>
+  <si>
+    <t>FGHIJK</t>
+  </si>
+  <si>
+    <t>LMNOPQ</t>
+  </si>
+  <si>
+    <t>FHG1234$</t>
+  </si>
+  <si>
+    <t>pqrst123#</t>
+  </si>
+  <si>
+    <t>ErrContains</t>
+  </si>
+  <si>
+    <t>does not match</t>
   </si>
 </sst>
 </file>
@@ -127,9 +142,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -445,52 +459,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C516F4FC-C478-4728-AB76-2B3C7B40D4E1}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>44549</v>
-      </c>
-      <c r="C2" s="1">
-        <v>44612</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF04254-6F85-4060-A89F-E5E3C5EB37FC}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -498,58 +470,58 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -560,4 +532,63 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2175876D-0DAC-4436-9D50-54BE7A956874}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
few test cases added for att.com
</commit_message>
<xml_diff>
--- a/com.bankofamerica.com/src/test/resources/boaTestData.xlsx
+++ b/com.bankofamerica.com/src/test/resources/boaTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nahid\IdeaProjects\Team5WDESeleniumBootcamp\com.bankofamerica.com\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F5AD7F-B44C-4E6D-9EA5-3178BD316C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2C40D1-EB99-4631-A5A4-7E3F0ED7769A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{5B3D6E91-87A4-427A-B005-9C27CF189E9B}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>email</t>
   </si>
@@ -94,10 +94,13 @@
     <t>pqrst123#</t>
   </si>
   <si>
-    <t>ErrContains</t>
-  </si>
-  <si>
-    <t>does not match</t>
+    <t>ABCDE2</t>
+  </si>
+  <si>
+    <t>FGHIJK2</t>
+  </si>
+  <si>
+    <t>LMNO2</t>
   </si>
 </sst>
 </file>
@@ -460,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF04254-6F85-4060-A89F-E5E3C5EB37FC}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C11" sqref="C11:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,6 +525,46 @@
       </c>
       <c r="D4" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -536,56 +579,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2175876D-0DAC-4436-9D50-54BE7A956874}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>